<commit_message>
burndown chart by william
</commit_message>
<xml_diff>
--- a/Burndown Chart ICQ.xlsx
+++ b/Burndown Chart ICQ.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\aaa\tkppl\ICQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
     <t>Project</t>
   </si>
@@ -118,6 +118,15 @@
   </si>
   <si>
     <t>informasi chat history, emoticons, themes, moods, microblog</t>
+  </si>
+  <si>
+    <t>informasi cara install ICQ di Windows,Linux,mobile(Iphone)</t>
+  </si>
+  <si>
+    <t>informasi cara install ICQ di Mac,Mobile(Symbian),Mobile(Blackberry),Mobile(Windows Phone 7)</t>
+  </si>
+  <si>
+    <t>informasi cara install ICQ di Mobile(Android),Mobile(Java),Mobile(Windows Mobile),Mobile(Bada)</t>
   </si>
 </sst>
 </file>
@@ -470,43 +479,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>39</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36</c:v>
+                  <c:v>38.769230769230766</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33</c:v>
+                  <c:v>35.538461538461533</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>32.307692307692299</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27</c:v>
+                  <c:v>29.07692307692307</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24</c:v>
+                  <c:v>25.84615384615384</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21</c:v>
+                  <c:v>22.61538461538461</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18</c:v>
+                  <c:v>19.38461538461538</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>15</c:v>
+                  <c:v>16.15384615384615</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12</c:v>
+                  <c:v>12.92307692307692</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9</c:v>
+                  <c:v>9.6923076923076898</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6</c:v>
+                  <c:v>6.461538461538459</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3</c:v>
+                  <c:v>3.2307692307692282</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0</c:v>
@@ -659,37 +668,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>39</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>31</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>28</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>22</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>17</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>17</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>5</c:v>
@@ -714,11 +723,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="1260110960"/>
-        <c:axId val="1260108240"/>
+        <c:axId val="259922240"/>
+        <c:axId val="259922800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1260110960"/>
+        <c:axId val="259922240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -784,7 +793,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1260108240"/>
+        <c:crossAx val="259922800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -792,7 +801,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1260108240"/>
+        <c:axId val="259922800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -858,7 +867,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1260110960"/>
+        <c:crossAx val="259922240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1253,7 +1262,7 @@
   <dimension ref="B1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1665,7 +1674,9 @@
       <c r="C11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="E11" s="2">
         <v>4</v>
       </c>
@@ -1716,36 +1727,38 @@
       <c r="C12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="D12" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="E12" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F12" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G12" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H12" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I12" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J12" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K12" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L12" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M12" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O12" s="2">
         <v>0</v>
@@ -1767,39 +1780,41 @@
       <c r="C13" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="E13" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F13" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G13" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H13" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I13" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J13" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K13" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L13" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M13" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N13" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="O13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P13" s="2">
         <v>0</v>
@@ -1972,55 +1987,55 @@
       <c r="D17" s="8"/>
       <c r="E17" s="2">
         <f>SUM(E5:E16)</f>
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F17" s="2">
         <f>E17-$E$17/13</f>
-        <v>36</v>
+        <v>38.769230769230766</v>
       </c>
       <c r="G17" s="2">
         <f>F17-$E$17/13</f>
-        <v>33</v>
+        <v>35.538461538461533</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" ref="H17:R17" si="0">G17-$E$17/13</f>
-        <v>30</v>
+        <v>32.307692307692299</v>
       </c>
       <c r="I17" s="2">
         <f t="shared" si="0"/>
-        <v>27</v>
+        <v>29.07692307692307</v>
       </c>
       <c r="J17" s="2">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>25.84615384615384</v>
       </c>
       <c r="K17" s="2">
         <f t="shared" si="0"/>
-        <v>21</v>
+        <v>22.61538461538461</v>
       </c>
       <c r="L17" s="2">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>19.38461538461538</v>
       </c>
       <c r="M17" s="2">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>16.15384615384615</v>
       </c>
       <c r="N17" s="2">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>12.92307692307692</v>
       </c>
       <c r="O17" s="2">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>9.6923076923076898</v>
       </c>
       <c r="P17" s="2">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>6.461538461538459</v>
       </c>
       <c r="Q17" s="2">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>3.2307692307692282</v>
       </c>
       <c r="R17" s="2">
         <f t="shared" si="0"/>
@@ -2035,47 +2050,47 @@
       <c r="D18" s="8"/>
       <c r="E18" s="2">
         <f>SUM(E2:E16)</f>
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="F18" s="2">
         <f>SUM(F5:F16)</f>
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G18" s="2">
         <f t="shared" ref="G18:R18" si="1">SUM(G5:G16)</f>
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H18" s="2">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="I18" s="2">
         <f t="shared" si="1"/>
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="J18" s="2">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="K18" s="2">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="L18" s="2">
         <f t="shared" si="1"/>
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="M18" s="2">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="N18" s="2">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="O18" s="2">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="P18" s="2">
         <f t="shared" si="1"/>

</xml_diff>